<commit_message>
Test inputs & outputs
</commit_message>
<xml_diff>
--- a/output/test.xlsx
+++ b/output/test.xlsx
@@ -403,7 +403,7 @@
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -432,7 +432,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>